<commit_message>
Login func started, create account func almost done, added userame and password to customer table
</commit_message>
<xml_diff>
--- a/spaceshiptabeller.xlsx
+++ b/spaceshiptabeller.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Documents\Medieinstitutet\Systemutveckling\Projekt\Enskild inlämningsuppgift\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projects\spaceship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E84BB1EB-D4F3-426C-9B35-CA0EAE8C703C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBCD705-5397-4846-8B96-F23906861E60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" xr2:uid="{FB61F1C7-BF72-4F6C-AED0-27C99F8A1179}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>Tabeller</t>
   </si>
@@ -127,6 +126,15 @@
   </si>
   <si>
     <t>4 st</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>PassWord</t>
+  </si>
+  <si>
+    <t>CHAR(128)</t>
   </si>
 </sst>
 </file>
@@ -515,7 +523,7 @@
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -661,8 +669,12 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
@@ -700,8 +712,12 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>

</xml_diff>